<commit_message>
Started aading components schematics to PumaTX KiCAD's library
</commit_message>
<xml_diff>
--- a/Organisation/ESP32 HSIS.xlsx
+++ b/Organisation/ESP32 HSIS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive\Bureau\PumaTX\Organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5470620-3B8B-435F-8AA1-C89EE707461B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4A8BBD-8658-4402-A2FB-5C7D5E824F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="23295" windowHeight="13740" activeTab="1" xr2:uid="{1B1BA6A8-BEBA-4A32-BD94-6781519408E2}"/>
+    <workbookView xWindow="12630" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{1B1BA6A8-BEBA-4A32-BD94-6781519408E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout usage" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>ESP32</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>TwoWire Wire1 = TwoWire(1);</t>
+  </si>
+  <si>
+    <t>Wifi antenna</t>
   </si>
 </sst>
 </file>
@@ -473,9 +476,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -485,110 +485,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -596,6 +497,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,51 +926,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="54"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="59"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U8" s="55" t="s">
+      <c r="U8" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="V8" s="56"/>
-      <c r="W8" s="57"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U9" s="58"/>
-      <c r="V9" s="59"/>
-      <c r="W9" s="60"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="65"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="39"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="44"/>
       <c r="U10" s="5" t="s">
         <v>2</v>
       </c>
@@ -982,10 +985,10 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K11" s="40"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="42"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="47"/>
       <c r="U11" s="5" t="s">
         <v>3</v>
       </c>
@@ -1000,10 +1003,10 @@
       <c r="Z11" s="6"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K12" s="40"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="42"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="47"/>
       <c r="U12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1018,10 +1021,10 @@
       <c r="Z12" s="6"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K13" s="40"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="42"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="47"/>
       <c r="U13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1036,10 +1039,10 @@
       <c r="Z13" s="6"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K14" s="40"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="47"/>
       <c r="U14" s="12" t="s">
         <v>5</v>
       </c>
@@ -1054,10 +1057,10 @@
       <c r="Z14" s="6"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K15" s="40"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="47"/>
       <c r="U15" s="5" t="s">
         <v>6</v>
       </c>
@@ -1072,10 +1075,10 @@
       <c r="Z15" s="6"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K16" s="40"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="42"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="47"/>
       <c r="U16" s="5" t="s">
         <v>7</v>
       </c>
@@ -1090,10 +1093,10 @@
       <c r="Z16" s="6"/>
     </row>
     <row r="17" spans="11:26" x14ac:dyDescent="0.25">
-      <c r="K17" s="40"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="42"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="47"/>
       <c r="U17" s="5" t="s">
         <v>8</v>
       </c>
@@ -1108,10 +1111,10 @@
       <c r="Z17" s="6"/>
     </row>
     <row r="18" spans="11:26" x14ac:dyDescent="0.25">
-      <c r="K18" s="40"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="42"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="47"/>
       <c r="U18" s="5" t="s">
         <v>12</v>
       </c>
@@ -1126,10 +1129,10 @@
       <c r="Z18" s="6"/>
     </row>
     <row r="19" spans="11:26" x14ac:dyDescent="0.25">
-      <c r="K19" s="40"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="42"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="47"/>
       <c r="U19" s="5" t="s">
         <v>14</v>
       </c>
@@ -1144,10 +1147,10 @@
       <c r="Z19" s="6"/>
     </row>
     <row r="20" spans="11:26" x14ac:dyDescent="0.25">
-      <c r="K20" s="40"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="42"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="47"/>
       <c r="U20" s="5"/>
       <c r="V20" s="6"/>
       <c r="W20" s="7"/>
@@ -1156,10 +1159,10 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="11:26" x14ac:dyDescent="0.25">
-      <c r="K21" s="40"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="42"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="47"/>
       <c r="U21" s="5"/>
       <c r="V21" s="6"/>
       <c r="W21" s="7"/>
@@ -1168,10 +1171,10 @@
       <c r="Z21" s="6"/>
     </row>
     <row r="22" spans="11:26" x14ac:dyDescent="0.25">
-      <c r="K22" s="40"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="42"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="47"/>
       <c r="U22" s="5"/>
       <c r="V22" s="6"/>
       <c r="W22" s="7"/>
@@ -1180,10 +1183,10 @@
       <c r="Z22" s="6"/>
     </row>
     <row r="23" spans="11:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K23" s="43"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="45"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="50"/>
       <c r="U23" s="5"/>
       <c r="V23" s="6"/>
       <c r="W23" s="7"/>
@@ -1222,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDA41B1-7788-4E76-9442-24D70B977B2C}">
   <dimension ref="A1:AD57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,27 +1236,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="48"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="56"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
       <c r="AA3" t="s">
         <v>45</v>
       </c>
@@ -1271,11 +1274,11 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="K5" s="69" t="s">
+      <c r="K5" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="70"/>
-      <c r="M5" s="71"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="69"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -1296,29 +1299,29 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="K7" s="5"/>
-      <c r="L7" s="55" t="s">
+      <c r="L7" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="57"/>
+      <c r="M7" s="62"/>
       <c r="N7" s="13" t="s">
         <v>25</v>
       </c>
       <c r="O7" s="6"/>
-      <c r="P7" s="55" t="s">
+      <c r="P7" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="57"/>
+      <c r="Q7" s="62"/>
       <c r="R7" s="13"/>
       <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="5"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="65"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="67"/>
       <c r="N8" s="17"/>
       <c r="O8" s="6"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="60"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="65"/>
       <c r="R8" s="14"/>
       <c r="S8" s="7"/>
     </row>
@@ -1344,10 +1347,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="62"/>
+      <c r="E10" s="72"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="4"/>
@@ -1364,11 +1367,11 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="7"/>
-      <c r="U10" s="61" t="s">
+      <c r="U10" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="V10" s="63"/>
-      <c r="W10" s="62"/>
+      <c r="V10" s="73"/>
+      <c r="W10" s="72"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="4"/>
     </row>
@@ -1411,10 +1414,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="57"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="13"/>
       <c r="H12" s="7"/>
       <c r="K12" s="8"/>
@@ -1427,10 +1430,10 @@
       <c r="R12" s="9"/>
       <c r="S12" s="10"/>
       <c r="U12" s="5"/>
-      <c r="V12" s="55" t="s">
+      <c r="V12" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="W12" s="57"/>
+      <c r="W12" s="62"/>
       <c r="X12" s="13"/>
       <c r="Y12" s="7"/>
     </row>
@@ -1442,16 +1445,16 @@
         <v>2</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="60"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="14">
         <v>7</v>
       </c>
       <c r="H13" s="7"/>
       <c r="K13" s="6"/>
       <c r="U13" s="5"/>
-      <c r="V13" s="58"/>
-      <c r="W13" s="60"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="65"/>
       <c r="X13" s="14">
         <v>12</v>
       </c>
@@ -1636,7 +1639,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="36" t="s">
+      <c r="L20" s="35" t="s">
         <v>46</v>
       </c>
       <c r="M20" s="31"/>
@@ -1717,10 +1720,10 @@
       <c r="K23" s="6"/>
       <c r="L23" s="30"/>
       <c r="M23" s="31"/>
-      <c r="N23" s="66" t="s">
+      <c r="N23" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="O23" s="66"/>
+      <c r="O23" s="70"/>
       <c r="P23" s="31"/>
       <c r="Q23" s="32"/>
       <c r="U23" s="5"/>
@@ -1738,15 +1741,15 @@
       <c r="K24" s="6"/>
       <c r="L24" s="30"/>
       <c r="M24" s="31"/>
-      <c r="N24" s="66"/>
-      <c r="O24" s="66"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="70"/>
       <c r="P24" s="31"/>
       <c r="Q24" s="32"/>
       <c r="U24" s="5"/>
-      <c r="V24" s="55" t="s">
+      <c r="V24" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="W24" s="57"/>
+      <c r="W24" s="62"/>
       <c r="X24" s="13" t="s">
         <v>25</v>
       </c>
@@ -1761,29 +1764,29 @@
       <c r="K25" s="6"/>
       <c r="L25" s="30"/>
       <c r="M25" s="31"/>
-      <c r="N25" s="66"/>
-      <c r="O25" s="66"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="70"/>
       <c r="P25" s="31"/>
       <c r="Q25" s="32"/>
       <c r="U25" s="5"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="65"/>
+      <c r="V25" s="66"/>
+      <c r="W25" s="67"/>
       <c r="X25" s="17"/>
       <c r="Y25" s="7"/>
     </row>
     <row r="26" spans="4:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
-      <c r="E26" s="55" t="s">
+      <c r="E26" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="57"/>
+      <c r="F26" s="62"/>
       <c r="G26" s="13"/>
       <c r="H26" s="7"/>
       <c r="K26" s="6"/>
       <c r="L26" s="30"/>
       <c r="M26" s="31"/>
-      <c r="N26" s="66"/>
-      <c r="O26" s="66"/>
+      <c r="N26" s="70"/>
+      <c r="O26" s="70"/>
       <c r="P26" s="31"/>
       <c r="Q26" s="32"/>
       <c r="U26" s="5"/>
@@ -1798,8 +1801,8 @@
     </row>
     <row r="27" spans="4:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="5"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="60"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="65"/>
       <c r="G27" s="14">
         <v>7</v>
       </c>
@@ -1807,10 +1810,10 @@
       <c r="K27" s="6"/>
       <c r="L27" s="30"/>
       <c r="M27" s="31"/>
-      <c r="N27" s="66"/>
-      <c r="O27" s="66"/>
+      <c r="N27" s="70"/>
+      <c r="O27" s="70"/>
       <c r="P27" s="31"/>
-      <c r="Q27" s="67" t="s">
+      <c r="Q27" s="36" t="s">
         <v>51</v>
       </c>
       <c r="U27" s="5"/>
@@ -1866,10 +1869,10 @@
       <c r="P29" s="31"/>
       <c r="Q29" s="32"/>
       <c r="U29" s="5"/>
-      <c r="V29" s="55" t="s">
+      <c r="V29" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="W29" s="57"/>
+      <c r="W29" s="62"/>
       <c r="X29" s="13" t="s">
         <v>25</v>
       </c>
@@ -1893,8 +1896,8 @@
       <c r="P30" s="31"/>
       <c r="Q30" s="32"/>
       <c r="U30" s="5"/>
-      <c r="V30" s="64"/>
-      <c r="W30" s="65"/>
+      <c r="V30" s="66"/>
+      <c r="W30" s="67"/>
       <c r="X30" s="17"/>
       <c r="Y30" s="7"/>
     </row>
@@ -1986,14 +1989,16 @@
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="K34" s="6"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="68"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="34"/>
-      <c r="P34" s="68" t="s">
+      <c r="L34" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="M34" s="37"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="Q34" s="35"/>
+      <c r="Q34" s="34"/>
       <c r="U34" s="8"/>
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
@@ -2062,11 +2067,11 @@
       <c r="S40" s="6"/>
     </row>
     <row r="41" spans="4:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K41" s="69" t="s">
+      <c r="K41" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="L41" s="71"/>
-      <c r="M41" s="72"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="38"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
@@ -2087,16 +2092,16 @@
     </row>
     <row r="43" spans="4:27" x14ac:dyDescent="0.25">
       <c r="K43" s="5"/>
-      <c r="L43" s="55" t="s">
+      <c r="L43" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="M43" s="57"/>
+      <c r="M43" s="62"/>
       <c r="N43" s="13"/>
       <c r="O43" s="6"/>
-      <c r="P43" s="55" t="s">
+      <c r="P43" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="Q43" s="57"/>
+      <c r="Q43" s="62"/>
       <c r="R43" s="13"/>
       <c r="S43" s="7"/>
       <c r="W43" t="s">
@@ -2105,12 +2110,12 @@
     </row>
     <row r="44" spans="4:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K44" s="5"/>
-      <c r="L44" s="64"/>
-      <c r="M44" s="65"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="67"/>
       <c r="N44" s="17"/>
       <c r="O44" s="6"/>
-      <c r="P44" s="58"/>
-      <c r="Q44" s="60"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="65"/>
       <c r="R44" s="14"/>
       <c r="S44" s="7"/>
       <c r="W44" t="s">
@@ -2120,11 +2125,11 @@
     <row r="45" spans="4:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K45" s="5"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="73"/>
+      <c r="M45" s="39"/>
       <c r="N45" s="4"/>
       <c r="O45" s="6"/>
       <c r="P45" s="15"/>
-      <c r="Q45" s="75"/>
+      <c r="Q45" s="41"/>
       <c r="R45" s="16"/>
       <c r="S45" s="7"/>
     </row>
@@ -2142,7 +2147,7 @@
     <row r="47" spans="4:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K47" s="5"/>
       <c r="L47" s="8"/>
-      <c r="M47" s="74"/>
+      <c r="M47" s="40"/>
       <c r="N47" s="10"/>
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
@@ -2153,7 +2158,7 @@
     <row r="48" spans="4:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K48" s="8"/>
       <c r="L48" s="9"/>
-      <c r="M48" s="74"/>
+      <c r="M48" s="40"/>
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
       <c r="P48" s="9"/>

</xml_diff>